<commit_message>
Reshape of comparison tables
</commit_message>
<xml_diff>
--- a/Tables/model_comparison_TANK_EFFECT.xlsx
+++ b/Tables/model_comparison_TANK_EFFECT.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Documents\KUL\Master thesis\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79BC7945-3673-4E1F-A981-C0BF42CCF9BA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF17BF2-C7FA-4C9A-BD87-7C6C996A40D4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D991A4A9-89F4-496F-94ED-18746D1539FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -65,7 +69,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="#,##0.000000"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -125,11 +129,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -139,7 +141,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -155,6 +159,44 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="FRESH_LS_SOLUTIONF"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="C3">
+            <v>1.3960624250110671</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="FRESH_RS_SOLUTIONF"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="C3">
+            <v>2.179024275658846</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -457,7 +499,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,81 +527,128 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="8">
         <v>2.952693</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="8">
         <v>3.7282380000000002</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="8">
         <v>0.21638755000000001</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="8">
         <v>0.2223098</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+      <c r="A3" s="5"/>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E3">
+      <c r="C3" s="8">
+        <f>C6+[1]FRESH_LS_SOLUTIONF!$C$3</f>
+        <v>2.7016367094544158</v>
+      </c>
+      <c r="D3" s="8">
+        <f>D6+[2]FRESH_RS_SOLUTIONF!$C$3</f>
+        <v>3.2975371760262329</v>
+      </c>
+      <c r="E3" s="8">
         <f>0.0415031953820438+0.165964640197899</f>
         <v>0.20746783557994281</v>
       </c>
+      <c r="F3" s="8">
+        <f>0.160602000231342+0.0353004770756604</f>
+        <v>0.19590247730700239</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+      <c r="A4" s="5"/>
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="C4" s="8">
+        <f>ABS(C2-C3)</f>
+        <v>0.2510562905455842</v>
+      </c>
+      <c r="D4" s="8">
+        <f t="shared" ref="D4:F4" si="0">ABS(D2-D3)</f>
+        <v>0.4307008239737673</v>
+      </c>
+      <c r="E4" s="8">
+        <f t="shared" si="0"/>
+        <v>8.9197144200572065E-3</v>
+      </c>
+      <c r="F4" s="8">
+        <f t="shared" si="0"/>
+        <v>2.6407322692997615E-2</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="9">
         <v>1.3342860000000001</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="9">
         <v>1.144482</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="9">
         <v>0.16218009999999999</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="9">
         <v>0.15226029999999999</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
+      <c r="A6" s="6"/>
       <c r="B6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6">
+      <c r="C6" s="8">
+        <v>1.3055742844433489</v>
+      </c>
+      <c r="D6" s="8">
+        <v>1.1185129003673866</v>
+      </c>
+      <c r="E6" s="8">
         <v>0.165964640197899</v>
+      </c>
+      <c r="F6" s="8">
+        <v>0.16060200023134166</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="5" t="s">
+      <c r="A7" s="7"/>
+      <c r="B7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
+      <c r="C7" s="10">
+        <f>ABS(C5-C6)</f>
+        <v>2.8711715556651196E-2</v>
+      </c>
+      <c r="D7" s="10">
+        <f t="shared" ref="D7:F7" si="1">ABS(D5-D6)</f>
+        <v>2.5969099632613402E-2</v>
+      </c>
+      <c r="E7" s="10">
+        <f t="shared" si="1"/>
+        <v>3.7845401978990056E-3</v>
+      </c>
+      <c r="F7" s="10">
+        <f t="shared" si="1"/>
+        <v>8.3417002313416755E-3</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>